<commit_message>
added results of spark and motor failure and cervical cancer data
</commit_message>
<xml_diff>
--- a/results_analysis/spark_motorFailure_02_hold_01_best.xlsx
+++ b/results_analysis/spark_motorFailure_02_hold_01_best.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\mltool_matlab_fp\results_analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\matlab-mltool-fp\results_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C8C8370-BF42-48ED-9CBF-A9605D958503}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB304A38-7E3E-4EC9-A388-C89D446030C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="734" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="734" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="acc_mean" sheetId="1" r:id="rId1"/>
@@ -143,8 +143,16 @@
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -519,7 +527,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -668,24 +676,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -705,6 +695,57 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -989,8 +1030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1008,19 +1049,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
     </row>
     <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1071,13 +1112,13 @@
       <c r="D5" s="42">
         <v>0.59605263157894794</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="63">
         <v>0.93361842105263204</v>
       </c>
       <c r="F5" s="12">
         <v>0.79256578947368395</v>
       </c>
-      <c r="G5" s="12">
+      <c r="G5" s="63">
         <v>0.93388157894736901</v>
       </c>
       <c r="H5" s="12">
@@ -1089,7 +1130,7 @@
       <c r="J5" s="12">
         <v>0.65690789473684197</v>
       </c>
-      <c r="K5" s="43">
+      <c r="K5" s="64">
         <v>0.93138157894736895</v>
       </c>
     </row>
@@ -1104,13 +1145,13 @@
       <c r="E6" s="13">
         <v>0.73947368421052595</v>
       </c>
-      <c r="F6" s="13">
+      <c r="F6" s="65">
         <v>0.79631578947368398</v>
       </c>
-      <c r="G6" s="13">
+      <c r="G6" s="65">
         <v>0.844342105263158</v>
       </c>
-      <c r="H6" s="13">
+      <c r="H6" s="65">
         <v>0.97256578947368399</v>
       </c>
       <c r="I6" s="13">
@@ -1134,7 +1175,7 @@
       <c r="D7" s="44">
         <v>0.67697368421052595</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="65">
         <v>0.93546052631578902</v>
       </c>
       <c r="F7" s="13">
@@ -1146,13 +1187,13 @@
       <c r="H7" s="13">
         <v>0.90355263157894805</v>
       </c>
-      <c r="I7" s="13">
+      <c r="I7" s="65">
         <v>0.91177631578947405</v>
       </c>
       <c r="J7" s="13">
         <v>0.60776315789473701</v>
       </c>
-      <c r="K7" s="15">
+      <c r="K7" s="66">
         <v>0.91703947368421102</v>
       </c>
     </row>
@@ -1171,10 +1212,10 @@
       <c r="F8" s="14">
         <v>0.79249999999999998</v>
       </c>
-      <c r="G8" s="14">
+      <c r="G8" s="67">
         <v>0.94552631578947399</v>
       </c>
-      <c r="H8" s="14">
+      <c r="H8" s="67">
         <v>0.97427631578947305</v>
       </c>
       <c r="I8" s="14">
@@ -1183,7 +1224,7 @@
       <c r="J8" s="14">
         <v>0.63809210526315796</v>
       </c>
-      <c r="K8" s="46">
+      <c r="K8" s="68">
         <v>0.99546052631578896</v>
       </c>
     </row>
@@ -1197,10 +1238,10 @@
       <c r="C9" s="3">
         <v>1</v>
       </c>
-      <c r="D9" s="47">
+      <c r="D9" s="70">
         <v>0.90881578947368502</v>
       </c>
-      <c r="E9" s="48">
+      <c r="E9" s="69">
         <v>0.936907894736842</v>
       </c>
       <c r="F9" s="48">
@@ -1212,7 +1253,7 @@
       <c r="H9" s="48">
         <v>0.89184210526315799</v>
       </c>
-      <c r="I9" s="48">
+      <c r="I9" s="69">
         <v>0.91789473684210598</v>
       </c>
       <c r="J9" s="48">
@@ -1233,16 +1274,16 @@
       <c r="E10" s="13">
         <v>0.70921052631578896</v>
       </c>
-      <c r="F10" s="13">
+      <c r="F10" s="65">
         <v>0.88717105263157903</v>
       </c>
       <c r="G10" s="13">
         <v>0.88131578947368405</v>
       </c>
-      <c r="H10" s="13">
+      <c r="H10" s="65">
         <v>0.98815789473684201</v>
       </c>
-      <c r="I10" s="13">
+      <c r="I10" s="65">
         <v>0.92105263157894701</v>
       </c>
       <c r="J10" s="13">
@@ -1269,16 +1310,16 @@
       <c r="F11" s="13">
         <v>0.85144736842105295</v>
       </c>
-      <c r="G11" s="13">
+      <c r="G11" s="65">
         <v>0.87276315789473702</v>
       </c>
       <c r="H11" s="13">
         <v>0.84789473684210503</v>
       </c>
-      <c r="I11" s="13">
+      <c r="I11" s="65">
         <v>0.91855263157894695</v>
       </c>
-      <c r="J11" s="13">
+      <c r="J11" s="65">
         <v>0.91355263157894695</v>
       </c>
       <c r="K11" s="15">
@@ -1291,7 +1332,7 @@
       <c r="C12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="45">
+      <c r="D12" s="71">
         <v>0.93164473684210503</v>
       </c>
       <c r="E12" s="14">
@@ -1300,10 +1341,10 @@
       <c r="F12" s="14">
         <v>0.924276315789474</v>
       </c>
-      <c r="G12" s="14">
+      <c r="G12" s="67">
         <v>0.96302631578947295</v>
       </c>
-      <c r="H12" s="14">
+      <c r="H12" s="67">
         <v>0.99671052631579005</v>
       </c>
       <c r="I12" s="14">
@@ -1326,28 +1367,28 @@
       <c r="C13" s="3">
         <v>1</v>
       </c>
-      <c r="D13" s="47">
+      <c r="D13" s="70">
         <v>0.89348684210526297</v>
       </c>
-      <c r="E13" s="48">
+      <c r="E13" s="69">
         <v>0.89249999999999996</v>
       </c>
       <c r="F13" s="48">
         <v>0.87855263157894703</v>
       </c>
-      <c r="G13" s="48">
+      <c r="G13" s="69">
         <v>0.89394736842105305</v>
       </c>
       <c r="H13" s="48">
         <v>0.89026315789473698</v>
       </c>
-      <c r="I13" s="48">
+      <c r="I13" s="69">
         <v>0.89651315789473696</v>
       </c>
       <c r="J13" s="48">
         <v>0.87124999999999997</v>
       </c>
-      <c r="K13" s="49">
+      <c r="K13" s="72">
         <v>0.89269736842105296</v>
       </c>
     </row>
@@ -1359,13 +1400,13 @@
       <c r="D14" s="44">
         <v>0.89335526315789504</v>
       </c>
-      <c r="E14" s="13">
+      <c r="E14" s="65">
         <v>0.99881578947368399</v>
       </c>
       <c r="F14" s="13">
         <v>0.89572368421052595</v>
       </c>
-      <c r="G14" s="13">
+      <c r="G14" s="65">
         <v>0.99776315789473702</v>
       </c>
       <c r="H14" s="13">
@@ -1377,7 +1418,7 @@
       <c r="J14" s="13">
         <v>0.85973684210526302</v>
       </c>
-      <c r="K14" s="15">
+      <c r="K14" s="66">
         <v>0.99802631578947398</v>
       </c>
     </row>
@@ -1389,7 +1430,7 @@
       <c r="C15" s="1">
         <v>1</v>
       </c>
-      <c r="D15" s="44">
+      <c r="D15" s="73">
         <v>0.89736842105263204</v>
       </c>
       <c r="E15" s="13">
@@ -1398,10 +1439,10 @@
       <c r="F15" s="13">
         <v>0.87782894736842099</v>
       </c>
-      <c r="G15" s="13">
+      <c r="G15" s="65">
         <v>0.89328947368421097</v>
       </c>
-      <c r="H15" s="13">
+      <c r="H15" s="65">
         <v>0.89453947368421105</v>
       </c>
       <c r="I15" s="13">
@@ -1423,13 +1464,13 @@
       <c r="D16" s="45">
         <v>0.893421052631579</v>
       </c>
-      <c r="E16" s="14">
+      <c r="E16" s="67">
         <v>0.999605263157895</v>
       </c>
       <c r="F16" s="14">
         <v>0.89710526315789496</v>
       </c>
-      <c r="G16" s="14">
+      <c r="G16" s="67">
         <v>0.99611842105263204</v>
       </c>
       <c r="H16" s="14">
@@ -1441,7 +1482,7 @@
       <c r="J16" s="14">
         <v>0.82743421052631605</v>
       </c>
-      <c r="K16" s="46">
+      <c r="K16" s="68">
         <v>0.99151315789473704</v>
       </c>
     </row>
@@ -1464,19 +1505,19 @@
       <c r="F17" s="48">
         <v>0.80236842105263195</v>
       </c>
-      <c r="G17" s="48">
+      <c r="G17" s="69">
         <v>0.93513157894736898</v>
       </c>
-      <c r="H17" s="48">
+      <c r="H17" s="69">
         <v>0.93427631578947401</v>
       </c>
-      <c r="I17" s="48">
+      <c r="I17" s="69">
         <v>0.93447368421052601</v>
       </c>
       <c r="J17" s="48">
         <v>0.64828947368420997</v>
       </c>
-      <c r="K17" s="49">
+      <c r="K17" s="72">
         <v>0.93500000000000005</v>
       </c>
     </row>
@@ -1497,16 +1538,16 @@
       <c r="G18" s="13">
         <v>0.91578947368421004</v>
       </c>
-      <c r="H18" s="13">
+      <c r="H18" s="65">
         <v>0.96223684210526295</v>
       </c>
-      <c r="I18" s="13">
+      <c r="I18" s="65">
         <v>0.93276315789473696</v>
       </c>
       <c r="J18" s="13">
         <v>0.66427631578947399</v>
       </c>
-      <c r="K18" s="15">
+      <c r="K18" s="66">
         <v>0.97835526315789401</v>
       </c>
     </row>
@@ -1527,10 +1568,10 @@
       <c r="F19" s="13">
         <v>0.88875000000000004</v>
       </c>
-      <c r="G19" s="13">
+      <c r="G19" s="65">
         <v>0.933289473684211</v>
       </c>
-      <c r="H19" s="13">
+      <c r="H19" s="65">
         <v>0.93526315789473702</v>
       </c>
       <c r="I19" s="13">
@@ -1539,7 +1580,7 @@
       <c r="J19" s="13">
         <v>0.70835526315789499</v>
       </c>
-      <c r="K19" s="15">
+      <c r="K19" s="66">
         <v>0.93578947368421095</v>
       </c>
     </row>
@@ -1558,10 +1599,10 @@
       <c r="F20" s="14">
         <v>0.75855263157894703</v>
       </c>
-      <c r="G20" s="14">
+      <c r="G20" s="67">
         <v>0.94059210526315795</v>
       </c>
-      <c r="H20" s="14">
+      <c r="H20" s="67">
         <v>0.95802631578947295</v>
       </c>
       <c r="I20" s="14">
@@ -1570,7 +1611,7 @@
       <c r="J20" s="14">
         <v>0.73848684210526305</v>
       </c>
-      <c r="K20" s="46">
+      <c r="K20" s="68">
         <v>0.96440789473684196</v>
       </c>
     </row>
@@ -1940,61 +1981,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="50"/>
-      <c r="N1" s="50"/>
-      <c r="O1" s="50"/>
-      <c r="P1" s="50"/>
-      <c r="Q1" s="50"/>
-      <c r="R1" s="50"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="57"/>
+      <c r="O1" s="57"/>
+      <c r="P1" s="57"/>
+      <c r="Q1" s="57"/>
+      <c r="R1" s="57"/>
     </row>
     <row r="2" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D3" s="55" t="s">
+      <c r="D3" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="53"/>
-      <c r="F3" s="52" t="s">
+      <c r="E3" s="60"/>
+      <c r="F3" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="53"/>
-      <c r="H3" s="52" t="s">
+      <c r="G3" s="60"/>
+      <c r="H3" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="53"/>
-      <c r="J3" s="52" t="s">
+      <c r="I3" s="60"/>
+      <c r="J3" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="53"/>
-      <c r="L3" s="52" t="s">
+      <c r="K3" s="60"/>
+      <c r="L3" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="M3" s="53"/>
-      <c r="N3" s="52" t="s">
+      <c r="M3" s="60"/>
+      <c r="N3" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="O3" s="53"/>
-      <c r="P3" s="52" t="s">
+      <c r="O3" s="60"/>
+      <c r="P3" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="Q3" s="53"/>
-      <c r="R3" s="52" t="s">
+      <c r="Q3" s="60"/>
+      <c r="R3" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="S3" s="54"/>
+      <c r="S3" s="61"/>
     </row>
     <row r="4" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
@@ -2065,7 +2106,7 @@
       <c r="C5" s="3">
         <v>1</v>
       </c>
-      <c r="D5" s="61">
+      <c r="D5" s="55">
         <v>0.25</v>
       </c>
       <c r="E5" s="27">
@@ -2077,7 +2118,7 @@
       <c r="G5" s="27">
         <v>1024.001</v>
       </c>
-      <c r="H5" s="62">
+      <c r="H5" s="56">
         <v>1</v>
       </c>
       <c r="I5" s="27">
@@ -2095,7 +2136,7 @@
       <c r="M5" s="27">
         <v>1024.001</v>
       </c>
-      <c r="N5" s="62">
+      <c r="N5" s="56">
         <v>-2</v>
       </c>
       <c r="O5" s="27">
@@ -3279,19 +3320,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
@@ -3882,19 +3923,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
@@ -4492,19 +4533,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
     </row>
     <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -5420,19 +5461,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
     </row>
     <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -6190,19 +6231,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
     </row>
     <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -7100,7 +7141,7 @@
   <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7118,19 +7159,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
     </row>
     <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -7888,19 +7929,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
     </row>
     <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -8639,8 +8680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F40056-F547-48DD-9331-37B657810592}">
   <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8658,19 +8699,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
     </row>
     <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -9428,19 +9469,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
     </row>
     <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -10200,24 +10241,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="50"/>
-      <c r="N1" s="50"/>
-      <c r="O1" s="50"/>
-      <c r="P1" s="50"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="57"/>
+      <c r="O1" s="57"/>
+      <c r="P1" s="57"/>
     </row>
     <row r="2" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -10227,29 +10268,29 @@
       <c r="E3" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="51" t="s">
+      <c r="F3" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="58"/>
       <c r="I3" s="18" t="s">
         <v>13</v>
       </c>
       <c r="J3" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="52" t="s">
+      <c r="K3" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="53"/>
-      <c r="M3" s="52" t="s">
+      <c r="L3" s="60"/>
+      <c r="M3" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="N3" s="53"/>
-      <c r="O3" s="52" t="s">
+      <c r="N3" s="60"/>
+      <c r="O3" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="P3" s="54"/>
+      <c r="P3" s="61"/>
     </row>
     <row r="4" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
@@ -10311,7 +10352,7 @@
       <c r="C5" s="21">
         <v>1</v>
       </c>
-      <c r="D5" s="56">
+      <c r="D5" s="50">
         <v>0</v>
       </c>
       <c r="E5" s="32">
@@ -10347,7 +10388,7 @@
       <c r="O5" s="33">
         <v>16</v>
       </c>
-      <c r="P5" s="59">
+      <c r="P5" s="53">
         <v>1</v>
       </c>
     </row>
@@ -10536,7 +10577,7 @@
       <c r="O9" s="13">
         <v>9.765625E-4</v>
       </c>
-      <c r="P9" s="60">
+      <c r="P9" s="54">
         <v>1</v>
       </c>
     </row>
@@ -10639,7 +10680,7 @@
       <c r="C12" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="57">
+      <c r="D12" s="51">
         <v>1</v>
       </c>
       <c r="E12" s="31">
@@ -10675,7 +10716,7 @@
       <c r="O12" s="29">
         <v>512</v>
       </c>
-      <c r="P12" s="60">
+      <c r="P12" s="54">
         <v>1</v>
       </c>
     </row>
@@ -11017,7 +11058,7 @@
       <c r="C20" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="58">
+      <c r="D20" s="52">
         <v>3.125E-2</v>
       </c>
       <c r="E20" s="38">

</xml_diff>

<commit_message>
small changes in excel file of motor failure
</commit_message>
<xml_diff>
--- a/results_analysis/spark_motorFailure_02_hold_01_best.xlsx
+++ b/results_analysis/spark_motorFailure_02_hold_01_best.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\mltool_matlab_fp\results_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9BDD82C-78C5-414C-9B56-2F4D26C0612E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E8AF844-F876-4C9D-9840-A7D28D339200}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="734" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="21840" windowHeight="13140" tabRatio="734" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="acc_mean" sheetId="1" r:id="rId1"/>
@@ -1083,7 +1083,7 @@
   <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+      <selection activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1879,7 +1879,7 @@
         <v>0.89736842105263204</v>
       </c>
       <c r="E28" s="87">
-        <v>0.999605263157895</v>
+        <v>0.999</v>
       </c>
       <c r="F28" s="73">
         <v>0.89710526315789496</v>

</xml_diff>